<commit_message>
tests and run main prog
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="45">
   <si>
     <t>Ticker</t>
   </si>
@@ -50,36 +50,54 @@
     <t>RUN</t>
   </si>
   <si>
+    <t>NET</t>
+  </si>
+  <si>
     <t>487.83M -&gt; 535.15M -&gt; 580.88M -&gt; 637.37M -&gt; 692.58M</t>
   </si>
   <si>
     <t>495.78M -&gt; 584.58M -&gt; 631.91M -&gt; 609.15M -&gt; 589.85M</t>
   </si>
   <si>
+    <t>212.17M -&gt; 234.52M -&gt; 253.86M -&gt; 274.7M -&gt; 290.18M</t>
+  </si>
+  <si>
     <t>-0.14 -&gt; -0.21 -&gt; -0.24 -&gt; -0.2 -&gt; 0.0</t>
   </si>
   <si>
     <t>-0.42 -&gt; -0.06 -&gt; 0.96 -&gt; 0.29 -&gt; -1.12</t>
   </si>
   <si>
+    <t>-0.13 -&gt; -0.2 -&gt; -0.13 -&gt; -0.14 -&gt; -0.12</t>
+  </si>
+  <si>
     <t>159.74M -&gt; 138.25M -&gt; 176.41M -&gt; 212.85M -&gt; 230.93M</t>
   </si>
   <si>
     <t>(683.51M) -&gt; (716.05M) -&gt; (636.94M) -&gt; (823.36M) -&gt; (949.63M)</t>
   </si>
   <si>
+    <t>(54.95M) -&gt; 6.65M -&gt; 6.13M -&gt; 34.08M -&gt; 20.81M</t>
+  </si>
+  <si>
     <t>1.61 &lt;- 1.22 &lt;- 2.19 &lt;- 3.79 &lt;- 4.63</t>
   </si>
   <si>
     <t>N/A &lt;- N/A &lt;- N/A &lt;- N/A</t>
   </si>
   <si>
+    <t>5.75 &lt;- N/A &lt;- N/A &lt;- N/A</t>
+  </si>
+  <si>
     <t>12.49 &lt;- 12.06 &lt;- 20.25 &lt;- 25.68 &lt;- 31.10</t>
   </si>
   <si>
     <t>1.90 &lt;- 2.41 &lt;- 2.95 &lt;- 2.73</t>
   </si>
   <si>
+    <t>20.63 &lt;- 16.39 &lt;- 21.85 &lt;- 18.96</t>
+  </si>
+  <si>
     <t>EPS Estimate</t>
   </si>
   <si>
@@ -104,22 +122,34 @@
     <t>-0.13</t>
   </si>
   <si>
+    <t>0.03</t>
+  </si>
+  <si>
     <t>0.57</t>
   </si>
   <si>
     <t>-1.12</t>
   </si>
   <si>
+    <t>0.08</t>
+  </si>
+  <si>
     <t>55900, 402</t>
   </si>
   <si>
     <t>83, -269</t>
   </si>
   <si>
+    <t>158, 157</t>
+  </si>
+  <si>
     <t>35, 35</t>
   </si>
   <si>
     <t>7, 8</t>
+  </si>
+  <si>
+    <t>30, 31</t>
   </si>
 </sst>
 </file>
@@ -492,7 +522,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -501,7 +531,7 @@
     <col min="1" max="1" width="6.7109375" customWidth="1"/>
     <col min="2" max="2" width="26.28515625" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="31.28515625" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
@@ -543,28 +573,28 @@
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2">
         <v>42</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E2" s="2">
         <v>100</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G2" s="2">
         <v>45</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" customHeight="1">
@@ -572,28 +602,57 @@
         <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3">
         <v>19</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E3" s="3">
         <v>-167</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G3" s="3">
         <v>-39</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="I3" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" customHeight="1">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2">
+        <v>37</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2">
+        <v>8</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="G4" s="2">
+        <v>138</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -603,7 +662,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -623,22 +682,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="30" customHeight="1">
@@ -646,19 +705,19 @@
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D2" s="2">
         <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="G2" s="2">
         <v>52</v>
@@ -669,22 +728,45 @@
         <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D3" s="3">
         <v>-761</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="G3" s="3">
         <v>-13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" customHeight="1">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="2">
+        <v>166</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="2">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix price change calculations
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="25">
   <si>
     <t>Ticker</t>
   </si>
@@ -44,40 +44,22 @@
     <t>Price/Sales</t>
   </si>
   <si>
-    <t>CRWD</t>
-  </si>
-  <si>
-    <t>NET</t>
-  </si>
-  <si>
-    <t>487.83M -&gt; 535.15M -&gt; 580.88M -&gt; 637.37M -&gt; 692.58M</t>
-  </si>
-  <si>
-    <t>212.17M -&gt; 234.52M -&gt; 253.86M -&gt; 274.7M -&gt; 290.18M</t>
-  </si>
-  <si>
-    <t>-0.14 -&gt; -0.21 -&gt; -0.24 -&gt; -0.2 -&gt; 0.0</t>
-  </si>
-  <si>
-    <t>-0.13 -&gt; -0.2 -&gt; -0.13 -&gt; -0.14 -&gt; -0.12</t>
-  </si>
-  <si>
-    <t>159.74M -&gt; 138.25M -&gt; 176.41M -&gt; 212.85M -&gt; 230.93M</t>
-  </si>
-  <si>
-    <t>(54.95M) -&gt; 6.65M -&gt; 6.13M -&gt; 34.08M -&gt; 20.81M</t>
-  </si>
-  <si>
-    <t>1.61 &lt;- 1.22 &lt;- 2.19 &lt;- 3.79 &lt;- 4.63</t>
-  </si>
-  <si>
-    <t>5.75 &lt;- N/A &lt;- N/A &lt;- N/A</t>
-  </si>
-  <si>
-    <t>12.49 &lt;- 12.06 &lt;- 20.25 &lt;- 25.68 &lt;- 31.10</t>
-  </si>
-  <si>
-    <t>20.63 &lt;- 16.39 &lt;- 21.85 &lt;- 18.96</t>
+    <t>TSLA</t>
+  </si>
+  <si>
+    <t>16.93B -&gt; 21.45B -&gt; 24.32B -&gt; 23.33B -&gt; 24.93B</t>
+  </si>
+  <si>
+    <t>0.65 -&gt; 0.95 -&gt; 1.07 -&gt; 0.73 -&gt; 0.78</t>
+  </si>
+  <si>
+    <t>621M -&gt; 3.3B -&gt; 1.42B -&gt; 427M -&gt; 1.01B</t>
+  </si>
+  <si>
+    <t>2.89 &lt;- 1.89 &lt;- 1.08 &lt;- 1.26 &lt;- 1.64</t>
+  </si>
+  <si>
+    <t>10.57 &lt;- 8.85 &lt;- 5.68 &lt;- 13.55 &lt;- 12.29</t>
   </si>
   <si>
     <t>EPS Estimate</t>
@@ -98,28 +80,16 @@
     <t>Price Delta</t>
   </si>
   <si>
-    <t>0.51</t>
-  </si>
-  <si>
-    <t>0.03</t>
-  </si>
-  <si>
-    <t>0.57</t>
-  </si>
-  <si>
-    <t>0.08</t>
-  </si>
-  <si>
-    <t>55900, 402</t>
-  </si>
-  <si>
-    <t>158, 157</t>
-  </si>
-  <si>
-    <t>35, 35</t>
-  </si>
-  <si>
-    <t>30, 31</t>
+    <t>0.75</t>
+  </si>
+  <si>
+    <t>0.82</t>
+  </si>
+  <si>
+    <t>-6, -13</t>
+  </si>
+  <si>
+    <t>4, 11</t>
   </si>
 </sst>
 </file>
@@ -142,7 +112,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,12 +122,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF4F9F8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -189,13 +153,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -492,21 +453,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="6.7109375" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
     <col min="8" max="8" width="21.7109375" customWidth="1"/>
-    <col min="9" max="9" width="21.28515625" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20" customHeight="1">
@@ -543,57 +504,28 @@
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2">
+        <v>47</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2">
-        <v>42</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2">
+        <v>20</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2">
+        <v>63</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="2">
-        <v>100</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="2">
-        <v>45</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="30" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="3">
-        <v>37</v>
-      </c>
-      <c r="D3" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="E3" s="3">
-        <v>8</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="3">
-        <v>138</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -603,7 +535,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -623,22 +555,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="30" customHeight="1">
@@ -646,45 +578,22 @@
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D2" s="2">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="G2" s="2">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="30" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="3">
-        <v>166</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="3">
-        <v>27</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update api code for ps/growth calc
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="27">
   <si>
     <t>Ticker</t>
   </si>
@@ -41,25 +41,31 @@
     <t>Price/Earnings/Growth</t>
   </si>
   <si>
+    <t>Price/Sales/Growth</t>
+  </si>
+  <si>
     <t>Price/Sales</t>
   </si>
   <si>
-    <t>TSLA</t>
-  </si>
-  <si>
-    <t>16.93B -&gt; 21.45B -&gt; 24.32B -&gt; 23.33B -&gt; 24.93B</t>
-  </si>
-  <si>
-    <t>0.65 -&gt; 0.95 -&gt; 1.07 -&gt; 0.73 -&gt; 0.78</t>
-  </si>
-  <si>
-    <t>621M -&gt; 3.3B -&gt; 1.42B -&gt; 427M -&gt; 1.01B</t>
-  </si>
-  <si>
-    <t>2.89 &lt;- 1.89 &lt;- 1.08 &lt;- 1.26 &lt;- 1.64</t>
-  </si>
-  <si>
-    <t>10.57 &lt;- 8.85 &lt;- 5.68 &lt;- 13.55 &lt;- 12.29</t>
+    <t>CRWD</t>
+  </si>
+  <si>
+    <t>580.88M -&gt; 637.37M -&gt; 692.58M -&gt; 731.63M -&gt; 786.01M</t>
+  </si>
+  <si>
+    <t>-0.24 -&gt; -0.2 -&gt; 0.0 -&gt; 0.04 -&gt; 0.11</t>
+  </si>
+  <si>
+    <t>174.08M -&gt; 209.53M -&gt; 227.73M -&gt; 189.29M -&gt; 239.62M</t>
+  </si>
+  <si>
+    <t>1.51 &lt;- 2.12 &lt;- 1.61 &lt;- 1.22 &lt;- 2.19</t>
+  </si>
+  <si>
+    <t>0.45457142857142857 &lt;- 0.44457142857142856 &lt;- 0.3568571428571429 &lt;- 0.3445714285714286 &lt;- 0.5785714285714286</t>
+  </si>
+  <si>
+    <t>15.91 &lt;- 15.56 &lt;- 12.49 &lt;- 12.06 &lt;- 20.25</t>
   </si>
   <si>
     <t>EPS Estimate</t>
@@ -80,16 +86,16 @@
     <t>Price Delta</t>
   </si>
   <si>
-    <t>0.75</t>
+    <t>0.74</t>
   </si>
   <si>
     <t>0.82</t>
   </si>
   <si>
-    <t>-6, -13</t>
-  </si>
-  <si>
-    <t>4, 11</t>
+    <t>645, 473</t>
+  </si>
+  <si>
+    <t>31, 37</t>
   </si>
 </sst>
 </file>
@@ -453,24 +459,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="6.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
     <col min="8" max="8" width="21.7109375" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" customWidth="1"/>
+    <col min="9" max="9" width="54.7109375" customWidth="1"/>
+    <col min="10" max="10" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20" customHeight="1">
+    <row r="1" spans="1:10" ht="20" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -498,34 +505,40 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1">
+    <row r="2" spans="1:10" ht="30" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2">
-        <v>20</v>
+        <v>146</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -555,45 +568,45 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="30" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G2" s="2">
-        <v>40</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
format float in psgq
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -47,25 +47,25 @@
     <t>Price/Sales</t>
   </si>
   <si>
-    <t>CRWD</t>
-  </si>
-  <si>
-    <t>580.88M -&gt; 637.37M -&gt; 692.58M -&gt; 731.63M -&gt; 786.01M</t>
-  </si>
-  <si>
-    <t>-0.24 -&gt; -0.2 -&gt; 0.0 -&gt; 0.04 -&gt; 0.11</t>
-  </si>
-  <si>
-    <t>174.08M -&gt; 209.53M -&gt; 227.73M -&gt; 189.29M -&gt; 239.62M</t>
-  </si>
-  <si>
-    <t>1.51 &lt;- 2.12 &lt;- 1.61 &lt;- 1.22 &lt;- 2.19</t>
-  </si>
-  <si>
-    <t>0.45457142857142857 &lt;- 0.44457142857142856 &lt;- 0.3568571428571429 &lt;- 0.3445714285714286 &lt;- 0.5785714285714286</t>
-  </si>
-  <si>
-    <t>15.91 &lt;- 15.56 &lt;- 12.49 &lt;- 12.06 &lt;- 20.25</t>
+    <t>DDOG</t>
+  </si>
+  <si>
+    <t>436.53M -&gt; 469.4M -&gt; 481.71M -&gt; 509.46M -&gt; 547.54M</t>
+  </si>
+  <si>
+    <t>-0.08 -&gt; -0.09 -&gt; -0.08 -&gt; -0.01 -&gt; 0.06</t>
+  </si>
+  <si>
+    <t>73.91M -&gt; 104.39M -&gt; 125.05M -&gt; 150.82M -&gt; 146.67M</t>
+  </si>
+  <si>
+    <t>1.31 &lt;- 2.05 &lt;- 1.69 &lt;- 1.12 &lt;- 1.49</t>
+  </si>
+  <si>
+    <t>0.61 &lt;- 0.70 &lt;- 0.55 &lt;- 0.60 &lt;- 0.85</t>
+  </si>
+  <si>
+    <t>15.30 &lt;- 17.38 &lt;- 13.68 &lt;- 15.07 &lt;- 21.34</t>
   </si>
   <si>
     <t>EPS Estimate</t>
@@ -86,16 +86,16 @@
     <t>Price Delta</t>
   </si>
   <si>
-    <t>0.74</t>
-  </si>
-  <si>
-    <t>0.82</t>
-  </si>
-  <si>
-    <t>645, 473</t>
-  </si>
-  <si>
-    <t>31, 37</t>
+    <t>0.34</t>
+  </si>
+  <si>
+    <t>0.45</t>
+  </si>
+  <si>
+    <t>633, 1056</t>
+  </si>
+  <si>
+    <t>21, 25</t>
   </si>
 </sst>
 </file>
@@ -466,14 +466,14 @@
   <sheetFormatPr defaultRowHeight="30" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="6.7109375" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
     <col min="8" max="8" width="21.7109375" customWidth="1"/>
-    <col min="9" max="9" width="54.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
     <col min="10" max="10" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -517,19 +517,19 @@
         <v>11</v>
       </c>
       <c r="C2" s="2">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="2">
-        <v>146</v>
+        <v>175</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="2">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>14</v>
@@ -597,7 +597,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="2">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>25</v>
@@ -606,7 +606,7 @@
         <v>26</v>
       </c>
       <c r="G2" s="2">
-        <v>72</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>